<commit_message>
merge Work and chart
</commit_message>
<xml_diff>
--- a/AR/app/Uploads/AR.xlsx
+++ b/AR/app/Uploads/AR.xlsx
@@ -440,19 +440,19 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:E10" ca="1" si="0">RANDBETWEEN(10,100)</f>
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -461,19 +461,19 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B10" ca="1" si="1">RANDBETWEEN(10,100)</f>
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -482,19 +482,19 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -503,19 +503,19 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -524,19 +524,19 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -545,19 +545,19 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -570,15 +570,15 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -587,19 +587,19 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -608,19 +608,19 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -663,19 +663,19 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:E10" ca="1" si="0">RANDBETWEEN(10,100)</f>
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -684,19 +684,19 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B10" ca="1" si="1">RANDBETWEEN(10,100)</f>
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -705,19 +705,19 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -726,19 +726,19 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -747,19 +747,19 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -768,19 +768,19 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -789,19 +789,19 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -810,19 +810,19 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -831,19 +831,19 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -856,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -885,19 +885,19 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(10,100)</f>
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:E10" ca="1" si="0">RANDBETWEEN(10,100)</f>
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -906,19 +906,19 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B10" ca="1" si="1">RANDBETWEEN(10,100)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -927,19 +927,19 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -948,15 +948,15 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
@@ -969,19 +969,19 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -990,19 +990,19 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1011,19 +1011,19 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1032,19 +1032,19 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1053,19 +1053,19 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="0"/>
         <v>33</v>
       </c>
-      <c r="D10">
-        <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>